<commit_message>
Bug fixing & features improvements
</commit_message>
<xml_diff>
--- a/public/fileStore/import_template/products_import_normal_template.xlsx
+++ b/public/fileStore/import_template/products_import_normal_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Little Pro\Desktop\APOTEk\apotek_systems_pos\public\fileStore\import_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{551E4467-A72A-4FDA-BB46-2851FDDEB5DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C5860D-A562-43E1-9D91-0C56D1C7B6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5E4D20C7-D269-441D-A8EC-D6C44E917C10}"/>
+    <workbookView xWindow="75" yWindow="780" windowWidth="20415" windowHeight="8190" xr2:uid="{5E4D20C7-D269-441D-A8EC-D6C44E917C10}"/>
   </bookViews>
   <sheets>
     <sheet name="product_import_template" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Mo cola</t>
   </si>
@@ -61,12 +61,6 @@
     </r>
   </si>
   <si>
-    <t>pack_size</t>
-  </si>
-  <si>
-    <t>brand</t>
-  </si>
-  <si>
     <t>barcode</t>
   </si>
   <si>
@@ -74,9 +68,6 @@
   </si>
   <si>
     <t>min_stock</t>
-  </si>
-  <si>
-    <t>max_stock</t>
   </si>
   <si>
     <r>
@@ -91,6 +82,9 @@
       </rPr>
       <t>*</t>
     </r>
+  </si>
+  <si>
+    <t>Dawa Mpya</t>
   </si>
 </sst>
 </file>
@@ -945,68 +939,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DEEFF03-B454-4866-8B40-EA869BDF4730}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" customWidth="1"/>
-    <col min="7" max="7" width="9" customWidth="1"/>
-    <col min="8" max="9" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100001</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="E2">
-        <v>300</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="C2">
+        <v>123456789</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="E2" t="s">
         <v>2</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>100002</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>111222333</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>